<commit_message>
sacando frecuencia entre 0 y 280hz
</commit_message>
<xml_diff>
--- a/jose/clasificador/fear2.xlsx
+++ b/jose/clasificador/fear2.xlsx
@@ -412,7 +412,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>662.3975461661881</v>
+        <v>200.7141250562303</v>
       </c>
       <c r="C2">
         <v>0.114904023706913</v>
@@ -430,7 +430,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0.5132869256050925</v>
+        <v>1.693951533828267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>